<commit_message>
Update Gantt diagrams to extend to November 30th
</commit_message>
<xml_diff>
--- a/docs/gantt.xlsx
+++ b/docs/gantt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Features</t>
   </si>
@@ -44,7 +44,28 @@
     <t>Multiple chat rooms</t>
   </si>
   <si>
-    <t>Final testing</t>
+    <t>Text chat</t>
+  </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
+    <t>Create database management</t>
+  </si>
+  <si>
+    <t>Implement accounts</t>
+  </si>
+  <si>
+    <t>Recorded sessions</t>
+  </si>
+  <si>
+    <t>Plan storage framework</t>
+  </si>
+  <si>
+    <t>Implement recording</t>
+  </si>
+  <si>
+    <t>Prototype testing</t>
   </si>
 </sst>
 </file>
@@ -88,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -96,16 +117,120 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0070C0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0070C0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0070C0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,18 +545,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:AT18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:U7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="46" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,8 +621,83 @@
       <c r="U1" s="1">
         <v>43044</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="1">
+        <v>43045</v>
+      </c>
+      <c r="W1" s="1">
+        <v>43046</v>
+      </c>
+      <c r="X1" s="1">
+        <v>43047</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>43048</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>43049</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>43050</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>43051</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>43052</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>43053</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>43054</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>43055</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>43056</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>43057</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>43058</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>43059</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>43060</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>43061</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>43062</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>43063</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>43064</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>43065</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>43066</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>43067</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>43068</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>43069</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -504,7 +705,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -520,7 +721,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -529,7 +730,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -541,7 +742,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -550,12 +751,94 @@
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V8" s="7"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="9"/>
+    </row>
+    <row r="9" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="9"/>
+    </row>
+    <row r="10" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="14"/>
+    </row>
+    <row r="11" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG11" s="12"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="14"/>
+    </row>
+    <row r="12" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM12" s="10"/>
+      <c r="AN12" s="11"/>
+      <c r="AO12" s="11"/>
+      <c r="AP12" s="8"/>
+      <c r="AQ12" s="8"/>
+      <c r="AR12" s="8"/>
+      <c r="AS12" s="8"/>
+      <c r="AT12" s="9"/>
+    </row>
+    <row r="13" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM13" s="12"/>
+      <c r="AN13" s="13"/>
+      <c r="AO13" s="14"/>
+    </row>
+    <row r="14" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP14" s="12"/>
+      <c r="AQ14" s="13"/>
+      <c r="AR14" s="13"/>
+      <c r="AS14" s="13"/>
+      <c r="AT14" s="14"/>
+    </row>
+    <row r="18" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>